<commit_message>
updated website as of 04/04
</commit_message>
<xml_diff>
--- a/scotland_covid_data.xlsx
+++ b/scotland_covid_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="1080" windowWidth="24660" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -110,7 +110,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -170,8 +170,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -187,8 +207,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -201,8 +241,14 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -210,6 +256,16 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -217,6 +273,16 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -546,18 +612,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X14"/>
+  <dimension ref="A1:AA14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AA14" sqref="A1:AA14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="44" customWidth="1"/>
     <col min="25" max="25" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:27">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -630,8 +697,17 @@
       <c r="X1" s="5">
         <v>199</v>
       </c>
+      <c r="Y1" s="6">
+        <v>221</v>
+      </c>
+      <c r="Z1" s="6">
+        <v>240</v>
+      </c>
+      <c r="AA1" s="6">
+        <v>254</v>
+      </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:27">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -704,8 +780,17 @@
       <c r="X2" s="2">
         <v>87</v>
       </c>
+      <c r="Y2" s="7">
+        <v>93</v>
+      </c>
+      <c r="Z2" s="7">
+        <v>100</v>
+      </c>
+      <c r="AA2" s="7">
+        <v>110</v>
+      </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:27">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -778,8 +863,17 @@
       <c r="X3" s="2">
         <v>100</v>
       </c>
+      <c r="Y3" s="7">
+        <v>104</v>
+      </c>
+      <c r="Z3" s="7">
+        <v>122</v>
+      </c>
+      <c r="AA3" s="7">
+        <v>127</v>
+      </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:27">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -852,8 +946,17 @@
       <c r="X4" s="2">
         <v>96</v>
       </c>
+      <c r="Y4" s="7">
+        <v>119</v>
+      </c>
+      <c r="Z4" s="7">
+        <v>147</v>
+      </c>
+      <c r="AA4" s="7">
+        <v>173</v>
+      </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:27">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -926,8 +1029,17 @@
       <c r="X5" s="2">
         <v>146</v>
       </c>
+      <c r="Y5" s="7">
+        <v>172</v>
+      </c>
+      <c r="Z5" s="7">
+        <v>189</v>
+      </c>
+      <c r="AA5" s="7">
+        <v>208</v>
+      </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:27">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -1000,8 +1112,17 @@
       <c r="X6" s="2">
         <v>108</v>
       </c>
+      <c r="Y6" s="7">
+        <v>128</v>
+      </c>
+      <c r="Z6" s="7">
+        <v>173</v>
+      </c>
+      <c r="AA6" s="7">
+        <v>177</v>
+      </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:27">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1074,8 +1195,17 @@
       <c r="X7" s="2">
         <v>632</v>
       </c>
+      <c r="Y7" s="7">
+        <v>682</v>
+      </c>
+      <c r="Z7" s="7">
+        <v>779</v>
+      </c>
+      <c r="AA7" s="7">
+        <v>851</v>
+      </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:27">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1148,8 +1278,17 @@
       <c r="X8" s="2">
         <v>58</v>
       </c>
+      <c r="Y8" s="7">
+        <v>65</v>
+      </c>
+      <c r="Z8" s="7">
+        <v>72</v>
+      </c>
+      <c r="AA8" s="7">
+        <v>85</v>
+      </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:27">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -1222,8 +1361,17 @@
       <c r="X9" s="2">
         <v>284</v>
       </c>
+      <c r="Y9" s="7">
+        <v>320</v>
+      </c>
+      <c r="Z9" s="7">
+        <v>377</v>
+      </c>
+      <c r="AA9" s="7">
+        <v>427</v>
+      </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:27">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -1296,8 +1444,17 @@
       <c r="X10" s="2">
         <v>311</v>
       </c>
+      <c r="Y10" s="7">
+        <v>356</v>
+      </c>
+      <c r="Z10" s="7">
+        <v>408</v>
+      </c>
+      <c r="AA10" s="7">
+        <v>476</v>
+      </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:27">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -1370,8 +1527,17 @@
       <c r="X11" s="2">
         <v>2</v>
       </c>
+      <c r="Y11" s="7">
+        <v>2</v>
+      </c>
+      <c r="Z11" s="7">
+        <v>2</v>
+      </c>
+      <c r="AA11" s="7">
+        <v>4</v>
+      </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:27">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -1444,8 +1610,17 @@
       <c r="X12" s="2">
         <v>30</v>
       </c>
+      <c r="Y12" s="7">
+        <v>30</v>
+      </c>
+      <c r="Z12" s="7">
+        <v>36</v>
+      </c>
+      <c r="AA12" s="7">
+        <v>40</v>
+      </c>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:27">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -1518,8 +1693,17 @@
       <c r="X13" s="2">
         <v>254</v>
       </c>
+      <c r="Y13" s="7">
+        <v>307</v>
+      </c>
+      <c r="Z13" s="7">
+        <v>353</v>
+      </c>
+      <c r="AA13" s="7">
+        <v>410</v>
+      </c>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:27">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -1590,6 +1774,15 @@
         <v>0</v>
       </c>
       <c r="X14" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y14" s="7">
+        <v>3</v>
+      </c>
+      <c r="Z14" s="7">
+        <v>3</v>
+      </c>
+      <c r="AA14" s="7">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated as of 05/04
</commit_message>
<xml_diff>
--- a/scotland_covid_data.xlsx
+++ b/scotland_covid_data.xlsx
@@ -191,8 +191,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -248,7 +254,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -266,6 +272,9 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -283,6 +292,9 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -612,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA14"/>
+  <dimension ref="A1:AB14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AA14" sqref="A1:AA14"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AB14" sqref="A1:AB14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -624,7 +636,7 @@
     <col min="25" max="25" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:28">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -706,8 +718,11 @@
       <c r="AA1" s="6">
         <v>254</v>
       </c>
+      <c r="AB1" s="6">
+        <v>267</v>
+      </c>
     </row>
-    <row r="2" spans="1:27">
+    <row r="2" spans="1:28">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -789,8 +804,11 @@
       <c r="AA2" s="7">
         <v>110</v>
       </c>
+      <c r="AB2" s="7">
+        <v>130</v>
+      </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:28">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -872,8 +890,11 @@
       <c r="AA3" s="7">
         <v>127</v>
       </c>
+      <c r="AB3" s="7">
+        <v>141</v>
+      </c>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:28">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -955,8 +976,11 @@
       <c r="AA4" s="7">
         <v>173</v>
       </c>
+      <c r="AB4" s="7">
+        <v>200</v>
+      </c>
     </row>
-    <row r="5" spans="1:27">
+    <row r="5" spans="1:28">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -1038,8 +1062,11 @@
       <c r="AA5" s="7">
         <v>208</v>
       </c>
+      <c r="AB5" s="7">
+        <v>226</v>
+      </c>
     </row>
-    <row r="6" spans="1:27">
+    <row r="6" spans="1:28">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -1121,8 +1148,11 @@
       <c r="AA6" s="7">
         <v>177</v>
       </c>
+      <c r="AB6" s="7">
+        <v>194</v>
+      </c>
     </row>
-    <row r="7" spans="1:27">
+    <row r="7" spans="1:28">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1204,8 +1234,11 @@
       <c r="AA7" s="7">
         <v>851</v>
       </c>
+      <c r="AB7" s="7">
+        <v>931</v>
+      </c>
     </row>
-    <row r="8" spans="1:27">
+    <row r="8" spans="1:28">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1287,8 +1320,11 @@
       <c r="AA8" s="7">
         <v>85</v>
       </c>
+      <c r="AB8" s="7">
+        <v>99</v>
+      </c>
     </row>
-    <row r="9" spans="1:27">
+    <row r="9" spans="1:28">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -1370,8 +1406,11 @@
       <c r="AA9" s="7">
         <v>427</v>
       </c>
+      <c r="AB9" s="7">
+        <v>478</v>
+      </c>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:28">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -1453,8 +1492,11 @@
       <c r="AA10" s="7">
         <v>476</v>
       </c>
+      <c r="AB10" s="7">
+        <v>534</v>
+      </c>
     </row>
-    <row r="11" spans="1:27">
+    <row r="11" spans="1:28">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -1536,8 +1578,11 @@
       <c r="AA11" s="7">
         <v>4</v>
       </c>
+      <c r="AB11" s="7">
+        <v>4</v>
+      </c>
     </row>
-    <row r="12" spans="1:27">
+    <row r="12" spans="1:28">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -1619,8 +1664,11 @@
       <c r="AA12" s="7">
         <v>40</v>
       </c>
+      <c r="AB12" s="7">
+        <v>41</v>
+      </c>
     </row>
-    <row r="13" spans="1:27">
+    <row r="13" spans="1:28">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -1702,8 +1750,11 @@
       <c r="AA13" s="7">
         <v>410</v>
       </c>
+      <c r="AB13" s="7">
+        <v>457</v>
+      </c>
     </row>
-    <row r="14" spans="1:27">
+    <row r="14" spans="1:28">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -1784,6 +1835,9 @@
       </c>
       <c r="AA14" s="7">
         <v>3</v>
+      </c>
+      <c r="AB14" s="7">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
up to date as of 28/04
</commit_message>
<xml_diff>
--- a/scotland_covid_data.xlsx
+++ b/scotland_covid_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19620" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="500" yWindow="1680" windowWidth="12800" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -107,27 +107,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -138,19 +123,6 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -168,17 +140,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color auto="1"/>
@@ -188,7 +149,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="65">
+  <cellStyleXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -254,28 +215,86 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="65">
+  <cellStyles count="129">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -308,6 +327,38 @@
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -340,6 +391,38 @@
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -669,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD14"/>
+  <dimension ref="A1:AY14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AD14"/>
+    <sheetView tabSelected="1" topLeftCell="AU1" workbookViewId="0">
+      <selection activeCell="AY9" sqref="AY9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -681,1292 +764,2174 @@
     <col min="25" max="25" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2">
+    <row r="1" spans="1:51">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
         <v>1</v>
       </c>
-      <c r="C1" s="2">
+      <c r="C1" s="1">
         <v>3</v>
       </c>
-      <c r="D1" s="2">
+      <c r="D1" s="1">
         <v>4</v>
       </c>
-      <c r="E1" s="2">
+      <c r="E1" s="1">
         <v>4</v>
       </c>
-      <c r="F1" s="2">
-        <v>6</v>
-      </c>
-      <c r="G1" s="2">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2">
+      <c r="F1" s="1">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1">
         <v>7</v>
       </c>
-      <c r="I1" s="2">
-        <v>6</v>
-      </c>
-      <c r="J1" s="2">
+      <c r="I1" s="1">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1">
         <v>9</v>
       </c>
-      <c r="K1" s="2">
+      <c r="K1" s="1">
         <v>12</v>
       </c>
-      <c r="L1" s="2">
+      <c r="L1" s="1">
         <v>16</v>
       </c>
-      <c r="M1" s="2">
+      <c r="M1" s="1">
         <v>21</v>
       </c>
-      <c r="N1" s="2">
+      <c r="N1" s="1">
         <v>25</v>
       </c>
-      <c r="O1" s="2">
+      <c r="O1" s="1">
         <v>34</v>
       </c>
-      <c r="P1" s="2">
+      <c r="P1" s="1">
         <v>41</v>
       </c>
-      <c r="Q1" s="2">
+      <c r="Q1" s="1">
         <v>57</v>
       </c>
-      <c r="R1" s="2">
+      <c r="R1" s="1">
         <v>74</v>
       </c>
-      <c r="S1" s="2">
+      <c r="S1" s="1">
         <v>75</v>
       </c>
-      <c r="T1" s="2">
+      <c r="T1" s="1">
         <v>90</v>
       </c>
-      <c r="U1" s="2">
+      <c r="U1" s="1">
         <v>108</v>
       </c>
-      <c r="V1" s="2">
+      <c r="V1" s="1">
         <v>154</v>
       </c>
-      <c r="W1" s="2">
+      <c r="W1" s="1">
         <v>177</v>
       </c>
-      <c r="X1" s="3">
+      <c r="X1" s="1">
         <v>199</v>
       </c>
-      <c r="Y1" s="4">
+      <c r="Y1" s="3">
         <v>221</v>
       </c>
-      <c r="Z1" s="4">
+      <c r="Z1" s="3">
         <v>240</v>
       </c>
-      <c r="AA1" s="4">
+      <c r="AA1" s="3">
         <v>254</v>
       </c>
-      <c r="AB1" s="4">
+      <c r="AB1" s="3">
         <v>267</v>
       </c>
-      <c r="AC1" s="4">
+      <c r="AC1" s="3">
         <v>288</v>
       </c>
-      <c r="AD1" s="4">
+      <c r="AD1" s="3">
         <v>296</v>
       </c>
+      <c r="AE1" s="3">
+        <v>312</v>
+      </c>
+      <c r="AF1" s="3">
+        <v>362</v>
+      </c>
+      <c r="AG1" s="3">
+        <v>364</v>
+      </c>
+      <c r="AH1" s="3">
+        <v>376</v>
+      </c>
+      <c r="AI1" s="3">
+        <v>390</v>
+      </c>
+      <c r="AJ1" s="3">
+        <v>390</v>
+      </c>
+      <c r="AK1" s="3">
+        <v>416</v>
+      </c>
+      <c r="AL1" s="3">
+        <v>457</v>
+      </c>
+      <c r="AM1" s="3">
+        <v>503</v>
+      </c>
+      <c r="AN1" s="3">
+        <v>536</v>
+      </c>
+      <c r="AO1" s="3">
+        <v>560</v>
+      </c>
+      <c r="AP1" s="3">
+        <v>586</v>
+      </c>
+      <c r="AQ1" s="3">
+        <v>604</v>
+      </c>
+      <c r="AR1" s="3">
+        <v>623</v>
+      </c>
+      <c r="AS1" s="3">
+        <v>640</v>
+      </c>
+      <c r="AT1" s="3">
+        <v>653</v>
+      </c>
+      <c r="AU1" s="3">
+        <v>678</v>
+      </c>
+      <c r="AV1" s="3">
+        <v>692</v>
+      </c>
+      <c r="AW1" s="3">
+        <v>705</v>
+      </c>
+      <c r="AX1" s="3">
+        <v>721</v>
+      </c>
+      <c r="AY1" s="3">
+        <v>738</v>
+      </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:51">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
-        <v>0</v>
-      </c>
-      <c r="C2" s="6">
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
         <v>2</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="2">
         <v>2</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="2">
         <v>3</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="2">
         <v>5</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="2">
         <v>7</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="2">
         <v>7</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="2">
         <v>7</v>
       </c>
-      <c r="J2" s="6">
+      <c r="J2" s="2">
         <v>7</v>
       </c>
-      <c r="K2" s="6">
+      <c r="K2" s="2">
         <v>8</v>
       </c>
-      <c r="L2" s="6">
+      <c r="L2" s="2">
         <v>9</v>
       </c>
-      <c r="M2" s="6">
+      <c r="M2" s="2">
         <v>10</v>
       </c>
-      <c r="N2" s="6">
+      <c r="N2" s="2">
         <v>11</v>
       </c>
-      <c r="O2" s="6">
+      <c r="O2" s="2">
         <v>12</v>
       </c>
-      <c r="P2" s="6">
+      <c r="P2" s="2">
         <v>12</v>
       </c>
-      <c r="Q2" s="6">
+      <c r="Q2" s="2">
         <v>15</v>
       </c>
-      <c r="R2" s="6">
+      <c r="R2" s="2">
         <v>23</v>
       </c>
-      <c r="S2" s="6">
+      <c r="S2" s="2">
         <v>28</v>
       </c>
-      <c r="T2" s="2">
+      <c r="T2" s="1">
         <v>35</v>
       </c>
-      <c r="U2" s="2">
+      <c r="U2" s="1">
         <v>50</v>
       </c>
-      <c r="V2" s="2">
+      <c r="V2" s="1">
         <v>63</v>
       </c>
-      <c r="W2" s="2">
+      <c r="W2" s="1">
         <v>77</v>
       </c>
-      <c r="X2" s="2">
+      <c r="X2" s="1">
         <v>87</v>
       </c>
-      <c r="Y2" s="7">
+      <c r="Y2" s="3">
         <v>93</v>
       </c>
-      <c r="Z2" s="7">
+      <c r="Z2" s="3">
         <v>100</v>
       </c>
-      <c r="AA2" s="7">
+      <c r="AA2" s="3">
         <v>110</v>
       </c>
-      <c r="AB2" s="7">
+      <c r="AB2" s="3">
         <v>130</v>
       </c>
-      <c r="AC2" s="7">
+      <c r="AC2" s="3">
         <v>139</v>
       </c>
-      <c r="AD2" s="7">
+      <c r="AD2" s="3">
         <v>149</v>
       </c>
+      <c r="AE2" s="3">
+        <v>160</v>
+      </c>
+      <c r="AF2" s="3">
+        <v>167</v>
+      </c>
+      <c r="AG2" s="3">
+        <v>177</v>
+      </c>
+      <c r="AH2" s="3">
+        <v>189</v>
+      </c>
+      <c r="AI2" s="3">
+        <v>199</v>
+      </c>
+      <c r="AJ2" s="3">
+        <v>204</v>
+      </c>
+      <c r="AK2" s="3">
+        <v>208</v>
+      </c>
+      <c r="AL2" s="3">
+        <v>215</v>
+      </c>
+      <c r="AM2" s="3">
+        <v>220</v>
+      </c>
+      <c r="AN2" s="3">
+        <v>229</v>
+      </c>
+      <c r="AO2" s="3">
+        <v>231</v>
+      </c>
+      <c r="AP2" s="3">
+        <v>237</v>
+      </c>
+      <c r="AQ2" s="3">
+        <v>239</v>
+      </c>
+      <c r="AR2" s="3">
+        <v>240</v>
+      </c>
+      <c r="AS2" s="3">
+        <v>243</v>
+      </c>
+      <c r="AT2" s="3">
+        <v>248</v>
+      </c>
+      <c r="AU2" s="3">
+        <v>253</v>
+      </c>
+      <c r="AV2" s="3">
+        <v>258</v>
+      </c>
+      <c r="AW2" s="3">
+        <v>259</v>
+      </c>
+      <c r="AX2" s="3">
+        <v>269</v>
+      </c>
+      <c r="AY2" s="3">
+        <v>272</v>
+      </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:51">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6">
-        <v>0</v>
-      </c>
-      <c r="C3" s="6">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6">
-        <v>0</v>
-      </c>
-      <c r="E3" s="6">
-        <v>0</v>
-      </c>
-      <c r="F3" s="6">
-        <v>0</v>
-      </c>
-      <c r="G3" s="6">
-        <v>0</v>
-      </c>
-      <c r="H3" s="6">
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
         <v>1</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="2">
         <v>1</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="2">
         <v>4</v>
       </c>
-      <c r="K3" s="6">
-        <v>6</v>
-      </c>
-      <c r="L3" s="6">
+      <c r="K3" s="2">
+        <v>6</v>
+      </c>
+      <c r="L3" s="2">
         <v>10</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="2">
         <v>13</v>
       </c>
-      <c r="N3" s="6">
+      <c r="N3" s="2">
         <v>16</v>
       </c>
-      <c r="O3" s="6">
+      <c r="O3" s="2">
         <v>18</v>
       </c>
-      <c r="P3" s="6">
+      <c r="P3" s="2">
         <v>26</v>
       </c>
-      <c r="Q3" s="6">
+      <c r="Q3" s="2">
         <v>31</v>
       </c>
-      <c r="R3" s="6">
+      <c r="R3" s="2">
         <v>39</v>
       </c>
-      <c r="S3" s="6">
+      <c r="S3" s="2">
         <v>47</v>
       </c>
-      <c r="T3" s="2">
+      <c r="T3" s="1">
         <v>60</v>
       </c>
-      <c r="U3" s="2">
+      <c r="U3" s="1">
         <v>63</v>
       </c>
-      <c r="V3" s="2">
+      <c r="V3" s="1">
         <v>74</v>
       </c>
-      <c r="W3" s="2">
+      <c r="W3" s="1">
         <v>92</v>
       </c>
-      <c r="X3" s="2">
+      <c r="X3" s="1">
         <v>100</v>
       </c>
-      <c r="Y3" s="7">
+      <c r="Y3" s="3">
         <v>104</v>
       </c>
-      <c r="Z3" s="7">
+      <c r="Z3" s="3">
         <v>122</v>
       </c>
-      <c r="AA3" s="7">
+      <c r="AA3" s="3">
         <v>127</v>
       </c>
-      <c r="AB3" s="7">
+      <c r="AB3" s="3">
         <v>141</v>
       </c>
-      <c r="AC3" s="7">
+      <c r="AC3" s="3">
         <v>144</v>
       </c>
-      <c r="AD3" s="7">
+      <c r="AD3" s="3">
         <v>152</v>
       </c>
+      <c r="AE3" s="3">
+        <v>155</v>
+      </c>
+      <c r="AF3" s="3">
+        <v>163</v>
+      </c>
+      <c r="AG3" s="3">
+        <v>164</v>
+      </c>
+      <c r="AH3" s="3">
+        <v>179</v>
+      </c>
+      <c r="AI3" s="3">
+        <v>186</v>
+      </c>
+      <c r="AJ3" s="3">
+        <v>192</v>
+      </c>
+      <c r="AK3" s="3">
+        <v>199</v>
+      </c>
+      <c r="AL3" s="3">
+        <v>207</v>
+      </c>
+      <c r="AM3" s="3">
+        <v>207</v>
+      </c>
+      <c r="AN3" s="3">
+        <v>209</v>
+      </c>
+      <c r="AO3" s="3">
+        <v>222</v>
+      </c>
+      <c r="AP3" s="3">
+        <v>229</v>
+      </c>
+      <c r="AQ3" s="3">
+        <v>231</v>
+      </c>
+      <c r="AR3" s="3">
+        <v>231</v>
+      </c>
+      <c r="AS3" s="3">
+        <v>235</v>
+      </c>
+      <c r="AT3" s="3">
+        <v>235</v>
+      </c>
+      <c r="AU3" s="3">
+        <v>235</v>
+      </c>
+      <c r="AV3" s="3">
+        <v>237</v>
+      </c>
+      <c r="AW3" s="3">
+        <v>240</v>
+      </c>
+      <c r="AX3" s="3">
+        <v>243</v>
+      </c>
+      <c r="AY3" s="3">
+        <v>243</v>
+      </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:51">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="2">
         <v>2</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="2">
         <v>2</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="2">
         <v>3</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="2">
         <v>4</v>
       </c>
-      <c r="F4" s="6">
-        <v>6</v>
-      </c>
-      <c r="G4" s="6">
+      <c r="F4" s="2">
+        <v>6</v>
+      </c>
+      <c r="G4" s="2">
         <v>7</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="2">
         <v>7</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="2">
         <v>7</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="2">
         <v>8</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="2">
         <v>9</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="2">
         <v>12</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="2">
         <v>13</v>
       </c>
-      <c r="N4" s="6">
+      <c r="N4" s="2">
         <v>16</v>
       </c>
-      <c r="O4" s="6">
+      <c r="O4" s="2">
         <v>19</v>
       </c>
-      <c r="P4" s="6">
+      <c r="P4" s="2">
         <v>25</v>
       </c>
-      <c r="Q4" s="6">
+      <c r="Q4" s="2">
         <v>29</v>
       </c>
-      <c r="R4" s="6">
+      <c r="R4" s="2">
         <v>40</v>
       </c>
-      <c r="S4" s="6">
+      <c r="S4" s="2">
         <v>41</v>
       </c>
-      <c r="T4" s="2">
+      <c r="T4" s="1">
         <v>51</v>
       </c>
-      <c r="U4" s="2">
+      <c r="U4" s="1">
         <v>58</v>
       </c>
-      <c r="V4" s="2">
+      <c r="V4" s="1">
         <v>70</v>
       </c>
-      <c r="W4" s="2">
+      <c r="W4" s="1">
         <v>76</v>
       </c>
-      <c r="X4" s="2">
+      <c r="X4" s="1">
         <v>96</v>
       </c>
-      <c r="Y4" s="7">
+      <c r="Y4" s="3">
         <v>119</v>
       </c>
-      <c r="Z4" s="7">
+      <c r="Z4" s="3">
         <v>147</v>
       </c>
-      <c r="AA4" s="7">
+      <c r="AA4" s="3">
         <v>173</v>
       </c>
-      <c r="AB4" s="7">
+      <c r="AB4" s="3">
         <v>200</v>
       </c>
-      <c r="AC4" s="7">
+      <c r="AC4" s="3">
         <v>227</v>
       </c>
-      <c r="AD4" s="7">
+      <c r="AD4" s="3">
         <v>239</v>
       </c>
+      <c r="AE4" s="3">
+        <v>255</v>
+      </c>
+      <c r="AF4" s="3">
+        <v>288</v>
+      </c>
+      <c r="AG4" s="3">
+        <v>133</v>
+      </c>
+      <c r="AH4" s="3">
+        <v>356</v>
+      </c>
+      <c r="AI4" s="3">
+        <v>379</v>
+      </c>
+      <c r="AJ4" s="3">
+        <v>383</v>
+      </c>
+      <c r="AK4" s="3">
+        <v>397</v>
+      </c>
+      <c r="AL4" s="3">
+        <v>424</v>
+      </c>
+      <c r="AM4" s="3">
+        <v>446</v>
+      </c>
+      <c r="AN4" s="3">
+        <v>488</v>
+      </c>
+      <c r="AO4" s="3">
+        <v>514</v>
+      </c>
+      <c r="AP4" s="3">
+        <v>532</v>
+      </c>
+      <c r="AQ4" s="3">
+        <v>542</v>
+      </c>
+      <c r="AR4" s="3">
+        <v>561</v>
+      </c>
+      <c r="AS4" s="3">
+        <v>593</v>
+      </c>
+      <c r="AT4" s="3">
+        <v>619</v>
+      </c>
+      <c r="AU4" s="3">
+        <v>637</v>
+      </c>
+      <c r="AV4" s="3">
+        <v>653</v>
+      </c>
+      <c r="AW4" s="3">
+        <v>672</v>
+      </c>
+      <c r="AX4" s="3">
+        <v>681</v>
+      </c>
+      <c r="AY4" s="3">
+        <v>692</v>
+      </c>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:51">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="2">
         <v>2</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="2">
         <v>2</v>
       </c>
-      <c r="D5" s="6">
-        <v>6</v>
-      </c>
-      <c r="E5" s="6">
-        <v>6</v>
-      </c>
-      <c r="F5" s="6">
-        <v>6</v>
-      </c>
-      <c r="G5" s="6">
+      <c r="D5" s="2">
+        <v>6</v>
+      </c>
+      <c r="E5" s="2">
+        <v>6</v>
+      </c>
+      <c r="F5" s="2">
+        <v>6</v>
+      </c>
+      <c r="G5" s="2">
         <v>10</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="2">
         <v>10</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="2">
         <v>12</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="2">
         <v>15</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="2">
         <v>17</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="2">
         <v>23</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="2">
         <v>27</v>
       </c>
-      <c r="N5" s="6">
+      <c r="N5" s="2">
         <v>30</v>
       </c>
-      <c r="O5" s="6">
+      <c r="O5" s="2">
         <v>40</v>
       </c>
-      <c r="P5" s="6">
+      <c r="P5" s="2">
         <v>43</v>
       </c>
-      <c r="Q5" s="6">
+      <c r="Q5" s="2">
         <v>59</v>
       </c>
-      <c r="R5" s="6">
+      <c r="R5" s="2">
         <v>75</v>
       </c>
-      <c r="S5" s="6">
+      <c r="S5" s="2">
         <v>81</v>
       </c>
-      <c r="T5" s="2">
+      <c r="T5" s="1">
         <v>95</v>
       </c>
-      <c r="U5" s="2">
+      <c r="U5" s="1">
         <v>94</v>
       </c>
-      <c r="V5" s="2">
+      <c r="V5" s="1">
         <v>103</v>
       </c>
-      <c r="W5" s="2">
+      <c r="W5" s="1">
         <v>131</v>
       </c>
-      <c r="X5" s="2">
+      <c r="X5" s="1">
         <v>146</v>
       </c>
-      <c r="Y5" s="7">
+      <c r="Y5" s="3">
         <v>172</v>
       </c>
-      <c r="Z5" s="7">
+      <c r="Z5" s="3">
         <v>189</v>
       </c>
-      <c r="AA5" s="7">
+      <c r="AA5" s="3">
         <v>208</v>
       </c>
-      <c r="AB5" s="7">
+      <c r="AB5" s="3">
         <v>226</v>
       </c>
-      <c r="AC5" s="7">
+      <c r="AC5" s="3">
         <v>231</v>
       </c>
-      <c r="AD5" s="7">
+      <c r="AD5" s="3">
         <v>243</v>
       </c>
+      <c r="AE5" s="3">
+        <v>259</v>
+      </c>
+      <c r="AF5" s="3">
+        <v>280</v>
+      </c>
+      <c r="AG5" s="3">
+        <v>302</v>
+      </c>
+      <c r="AH5" s="3">
+        <v>324</v>
+      </c>
+      <c r="AI5" s="3">
+        <v>337</v>
+      </c>
+      <c r="AJ5" s="3">
+        <v>352</v>
+      </c>
+      <c r="AK5" s="3">
+        <v>367</v>
+      </c>
+      <c r="AL5" s="3">
+        <v>380</v>
+      </c>
+      <c r="AM5" s="3">
+        <v>400</v>
+      </c>
+      <c r="AN5" s="3">
+        <v>431</v>
+      </c>
+      <c r="AO5" s="3">
+        <v>451</v>
+      </c>
+      <c r="AP5" s="3">
+        <v>509</v>
+      </c>
+      <c r="AQ5" s="3">
+        <v>542</v>
+      </c>
+      <c r="AR5" s="3">
+        <v>562</v>
+      </c>
+      <c r="AS5" s="3">
+        <v>569</v>
+      </c>
+      <c r="AT5" s="3">
+        <v>604</v>
+      </c>
+      <c r="AU5" s="3">
+        <v>606</v>
+      </c>
+      <c r="AV5" s="3">
+        <v>655</v>
+      </c>
+      <c r="AW5" s="3">
+        <v>662</v>
+      </c>
+      <c r="AX5" s="3">
+        <v>680</v>
+      </c>
+      <c r="AY5" s="3">
+        <v>689</v>
+      </c>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:51">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6">
-        <v>6</v>
-      </c>
-      <c r="C6" s="6">
-        <v>6</v>
-      </c>
-      <c r="D6" s="6">
+      <c r="B6" s="2">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2">
+        <v>6</v>
+      </c>
+      <c r="D6" s="2">
         <v>7</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="2">
         <v>11</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="2">
         <v>9</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="2">
         <v>12</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="2">
         <v>12</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="2">
         <v>22</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="2">
         <v>24</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="2">
         <v>18</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L6" s="2">
         <v>19</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="2">
         <v>20</v>
       </c>
-      <c r="N6" s="6">
+      <c r="N6" s="2">
         <v>23</v>
       </c>
-      <c r="O6" s="6">
+      <c r="O6" s="2">
         <v>24</v>
       </c>
-      <c r="P6" s="6">
+      <c r="P6" s="2">
         <v>24</v>
       </c>
-      <c r="Q6" s="6">
+      <c r="Q6" s="2">
         <v>29</v>
       </c>
-      <c r="R6" s="6">
+      <c r="R6" s="2">
         <v>31</v>
       </c>
-      <c r="S6" s="6">
+      <c r="S6" s="2">
         <v>45</v>
       </c>
-      <c r="T6" s="2">
+      <c r="T6" s="1">
         <v>52</v>
       </c>
-      <c r="U6" s="2">
+      <c r="U6" s="1">
         <v>62</v>
       </c>
-      <c r="V6" s="2">
+      <c r="V6" s="1">
         <v>66</v>
       </c>
-      <c r="W6" s="2">
+      <c r="W6" s="1">
         <v>86</v>
       </c>
-      <c r="X6" s="2">
+      <c r="X6" s="1">
         <v>108</v>
       </c>
-      <c r="Y6" s="7">
+      <c r="Y6" s="3">
         <v>128</v>
       </c>
-      <c r="Z6" s="7">
+      <c r="Z6" s="3">
         <v>173</v>
       </c>
-      <c r="AA6" s="7">
+      <c r="AA6" s="3">
         <v>177</v>
       </c>
-      <c r="AB6" s="7">
+      <c r="AB6" s="3">
         <v>194</v>
       </c>
-      <c r="AC6" s="7">
+      <c r="AC6" s="3">
         <v>209</v>
       </c>
-      <c r="AD6" s="7">
+      <c r="AD6" s="3">
         <v>210</v>
       </c>
+      <c r="AE6" s="3">
+        <v>223</v>
+      </c>
+      <c r="AF6" s="3">
+        <v>236</v>
+      </c>
+      <c r="AG6" s="3">
+        <v>251</v>
+      </c>
+      <c r="AH6" s="3">
+        <v>261</v>
+      </c>
+      <c r="AI6" s="3">
+        <v>291</v>
+      </c>
+      <c r="AJ6" s="3">
+        <v>313</v>
+      </c>
+      <c r="AK6" s="3">
+        <v>335</v>
+      </c>
+      <c r="AL6" s="3">
+        <v>257</v>
+      </c>
+      <c r="AM6" s="3">
+        <v>389</v>
+      </c>
+      <c r="AN6" s="3">
+        <v>394</v>
+      </c>
+      <c r="AO6" s="3">
+        <v>432</v>
+      </c>
+      <c r="AP6" s="3">
+        <v>464</v>
+      </c>
+      <c r="AQ6" s="3">
+        <v>490</v>
+      </c>
+      <c r="AR6" s="3">
+        <v>519</v>
+      </c>
+      <c r="AS6" s="3">
+        <v>550</v>
+      </c>
+      <c r="AT6" s="3">
+        <v>602</v>
+      </c>
+      <c r="AU6" s="3">
+        <v>638</v>
+      </c>
+      <c r="AV6" s="3">
+        <v>700</v>
+      </c>
+      <c r="AW6" s="3">
+        <v>748</v>
+      </c>
+      <c r="AX6" s="3">
+        <v>771</v>
+      </c>
+      <c r="AY6" s="3">
+        <v>782</v>
+      </c>
     </row>
-    <row r="7" spans="1:30">
+    <row r="7" spans="1:51">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="2">
         <v>3</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="2">
         <v>5</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="2">
         <v>10</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="2">
         <v>21</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="2">
         <v>31</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="2">
         <v>39</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="2">
         <v>44</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="2">
         <v>49</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="2">
         <v>57</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="2">
         <v>71</v>
       </c>
-      <c r="L7" s="6">
+      <c r="L7" s="2">
         <v>91</v>
       </c>
-      <c r="M7" s="6">
+      <c r="M7" s="2">
         <v>110</v>
       </c>
-      <c r="N7" s="6">
+      <c r="N7" s="2">
         <v>130</v>
       </c>
-      <c r="O7" s="6">
+      <c r="O7" s="2">
         <v>152</v>
       </c>
-      <c r="P7" s="6">
+      <c r="P7" s="2">
         <v>183</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="Q7" s="2">
         <v>221</v>
       </c>
-      <c r="R7" s="6">
+      <c r="R7" s="2">
         <v>258</v>
       </c>
-      <c r="S7" s="6">
+      <c r="S7" s="2">
         <v>299</v>
       </c>
-      <c r="T7" s="2">
+      <c r="T7" s="1">
         <v>376</v>
       </c>
-      <c r="U7" s="2">
+      <c r="U7" s="1">
         <v>401</v>
       </c>
-      <c r="V7" s="2">
+      <c r="V7" s="1">
         <v>449</v>
       </c>
-      <c r="W7" s="2">
+      <c r="W7" s="1">
         <v>547</v>
       </c>
-      <c r="X7" s="2">
+      <c r="X7" s="1">
         <v>632</v>
       </c>
-      <c r="Y7" s="7">
+      <c r="Y7" s="3">
         <v>682</v>
       </c>
-      <c r="Z7" s="7">
+      <c r="Z7" s="3">
         <v>779</v>
       </c>
-      <c r="AA7" s="7">
+      <c r="AA7" s="3">
         <v>851</v>
       </c>
-      <c r="AB7" s="7">
+      <c r="AB7" s="3">
         <v>931</v>
       </c>
-      <c r="AC7" s="7">
+      <c r="AC7" s="3">
         <v>984</v>
       </c>
-      <c r="AD7" s="7">
+      <c r="AD7" s="3">
         <v>1094</v>
       </c>
+      <c r="AE7" s="3">
+        <v>1166</v>
+      </c>
+      <c r="AF7" s="3">
+        <v>1251</v>
+      </c>
+      <c r="AG7" s="3">
+        <v>1314</v>
+      </c>
+      <c r="AH7" s="3">
+        <v>1387</v>
+      </c>
+      <c r="AI7" s="3">
+        <v>1449</v>
+      </c>
+      <c r="AJ7" s="3">
+        <v>1486</v>
+      </c>
+      <c r="AK7" s="3">
+        <v>1575</v>
+      </c>
+      <c r="AL7" s="3">
+        <v>1661</v>
+      </c>
+      <c r="AM7" s="3">
+        <v>1742</v>
+      </c>
+      <c r="AN7" s="3">
+        <v>1794</v>
+      </c>
+      <c r="AO7" s="3">
+        <v>1905</v>
+      </c>
+      <c r="AP7" s="3">
+        <v>1949</v>
+      </c>
+      <c r="AQ7" s="3">
+        <v>2020</v>
+      </c>
+      <c r="AR7" s="3">
+        <v>2085</v>
+      </c>
+      <c r="AS7" s="3">
+        <v>2174</v>
+      </c>
+      <c r="AT7" s="3">
+        <v>2250</v>
+      </c>
+      <c r="AU7" s="3">
+        <v>2311</v>
+      </c>
+      <c r="AV7" s="3">
+        <v>2428</v>
+      </c>
+      <c r="AW7" s="3">
+        <v>2479</v>
+      </c>
+      <c r="AX7" s="3">
+        <v>2531</v>
+      </c>
+      <c r="AY7" s="3">
+        <v>2604</v>
+      </c>
     </row>
-    <row r="8" spans="1:30">
+    <row r="8" spans="1:51">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="6">
-        <v>0</v>
-      </c>
-      <c r="C8" s="6">
-        <v>0</v>
-      </c>
-      <c r="D8" s="6">
-        <v>0</v>
-      </c>
-      <c r="E8" s="6">
-        <v>0</v>
-      </c>
-      <c r="F8" s="6">
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
         <v>1</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="2">
         <v>2</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="2">
         <v>2</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="2">
         <v>5</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="2">
         <v>5</v>
       </c>
-      <c r="K8" s="6">
-        <v>6</v>
-      </c>
-      <c r="L8" s="6">
-        <v>6</v>
-      </c>
-      <c r="M8" s="6">
+      <c r="K8" s="2">
+        <v>6</v>
+      </c>
+      <c r="L8" s="2">
+        <v>6</v>
+      </c>
+      <c r="M8" s="2">
         <v>8</v>
       </c>
-      <c r="N8" s="6">
+      <c r="N8" s="2">
         <v>8</v>
       </c>
-      <c r="O8" s="6">
+      <c r="O8" s="2">
         <v>12</v>
       </c>
-      <c r="P8" s="6">
+      <c r="P8" s="2">
         <v>13</v>
       </c>
-      <c r="Q8" s="6">
+      <c r="Q8" s="2">
         <v>22</v>
       </c>
-      <c r="R8" s="6">
+      <c r="R8" s="2">
         <v>29</v>
       </c>
-      <c r="S8" s="6">
+      <c r="S8" s="2">
         <v>33</v>
       </c>
-      <c r="T8" s="2">
+      <c r="T8" s="1">
         <v>36</v>
       </c>
-      <c r="U8" s="2">
+      <c r="U8" s="1">
         <v>42</v>
       </c>
-      <c r="V8" s="2">
+      <c r="V8" s="1">
         <v>44</v>
       </c>
-      <c r="W8" s="2">
+      <c r="W8" s="1">
         <v>51</v>
       </c>
-      <c r="X8" s="2">
+      <c r="X8" s="1">
         <v>58</v>
       </c>
-      <c r="Y8" s="7">
+      <c r="Y8" s="3">
         <v>65</v>
       </c>
-      <c r="Z8" s="7">
+      <c r="Z8" s="3">
         <v>72</v>
       </c>
-      <c r="AA8" s="7">
+      <c r="AA8" s="3">
         <v>85</v>
       </c>
-      <c r="AB8" s="7">
+      <c r="AB8" s="3">
         <v>99</v>
       </c>
-      <c r="AC8" s="7">
+      <c r="AC8" s="3">
         <v>102</v>
       </c>
-      <c r="AD8" s="7">
+      <c r="AD8" s="3">
         <v>112</v>
       </c>
+      <c r="AE8" s="3">
+        <v>122</v>
+      </c>
+      <c r="AF8" s="3">
+        <v>137</v>
+      </c>
+      <c r="AG8" s="3">
+        <v>144</v>
+      </c>
+      <c r="AH8" s="3">
+        <v>148</v>
+      </c>
+      <c r="AI8" s="3">
+        <v>151</v>
+      </c>
+      <c r="AJ8" s="3">
+        <v>163</v>
+      </c>
+      <c r="AK8" s="3">
+        <v>168</v>
+      </c>
+      <c r="AL8" s="3">
+        <v>180</v>
+      </c>
+      <c r="AM8" s="3">
+        <v>184</v>
+      </c>
+      <c r="AN8" s="3">
+        <v>187</v>
+      </c>
+      <c r="AO8" s="3">
+        <v>193</v>
+      </c>
+      <c r="AP8" s="3">
+        <v>197</v>
+      </c>
+      <c r="AQ8" s="3">
+        <v>198</v>
+      </c>
+      <c r="AR8" s="3">
+        <v>201</v>
+      </c>
+      <c r="AS8" s="3">
+        <v>211</v>
+      </c>
+      <c r="AT8" s="3">
+        <v>214</v>
+      </c>
+      <c r="AU8" s="3">
+        <v>214</v>
+      </c>
+      <c r="AV8" s="3">
+        <v>220</v>
+      </c>
+      <c r="AW8" s="3">
+        <v>225</v>
+      </c>
+      <c r="AX8" s="3">
+        <v>228</v>
+      </c>
+      <c r="AY8" s="3">
+        <v>232</v>
+      </c>
     </row>
-    <row r="9" spans="1:30">
+    <row r="9" spans="1:51">
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="2">
         <v>3</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="2">
         <v>4</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="2">
         <v>7</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="2">
         <v>7</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="2">
         <v>10</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="2">
         <v>16</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="2">
         <v>20</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="2">
         <v>21</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="2">
         <v>25</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K9" s="2">
         <v>33</v>
       </c>
-      <c r="L9" s="6">
+      <c r="L9" s="2">
         <v>41</v>
       </c>
-      <c r="M9" s="6">
+      <c r="M9" s="2">
         <v>49</v>
       </c>
-      <c r="N9" s="6">
+      <c r="N9" s="2">
         <v>49</v>
       </c>
-      <c r="O9" s="6">
+      <c r="O9" s="2">
         <v>58</v>
       </c>
-      <c r="P9" s="6">
+      <c r="P9" s="2">
         <v>75</v>
       </c>
-      <c r="Q9" s="6">
+      <c r="Q9" s="2">
         <v>87</v>
       </c>
-      <c r="R9" s="6">
+      <c r="R9" s="2">
         <v>114</v>
       </c>
-      <c r="S9" s="6">
+      <c r="S9" s="2">
         <v>140</v>
       </c>
-      <c r="T9" s="2">
+      <c r="T9" s="1">
         <v>165</v>
       </c>
-      <c r="U9" s="2">
+      <c r="U9" s="1">
         <v>184</v>
       </c>
-      <c r="V9" s="2">
+      <c r="V9" s="1">
         <v>197</v>
       </c>
-      <c r="W9" s="2">
+      <c r="W9" s="1">
         <v>244</v>
       </c>
-      <c r="X9" s="2">
+      <c r="X9" s="1">
         <v>284</v>
       </c>
-      <c r="Y9" s="7">
+      <c r="Y9" s="3">
         <v>320</v>
       </c>
-      <c r="Z9" s="7">
+      <c r="Z9" s="3">
         <v>377</v>
       </c>
-      <c r="AA9" s="7">
+      <c r="AA9" s="3">
         <v>427</v>
       </c>
-      <c r="AB9" s="7">
+      <c r="AB9" s="3">
         <v>478</v>
       </c>
-      <c r="AC9" s="7">
+      <c r="AC9" s="3">
         <v>512</v>
       </c>
-      <c r="AD9" s="7">
+      <c r="AD9" s="3">
         <v>547</v>
       </c>
+      <c r="AE9" s="3">
+        <v>575</v>
+      </c>
+      <c r="AF9" s="3">
+        <v>607</v>
+      </c>
+      <c r="AG9" s="3">
+        <v>662</v>
+      </c>
+      <c r="AH9" s="3">
+        <v>707</v>
+      </c>
+      <c r="AI9" s="3">
+        <v>758</v>
+      </c>
+      <c r="AJ9" s="3">
+        <v>784</v>
+      </c>
+      <c r="AK9" s="3">
+        <v>822</v>
+      </c>
+      <c r="AL9" s="3">
+        <v>873</v>
+      </c>
+      <c r="AM9" s="3">
+        <v>911</v>
+      </c>
+      <c r="AN9" s="3">
+        <v>934</v>
+      </c>
+      <c r="AO9" s="3">
+        <v>995</v>
+      </c>
+      <c r="AP9" s="3">
+        <v>1022</v>
+      </c>
+      <c r="AQ9" s="3">
+        <v>1051</v>
+      </c>
+      <c r="AR9" s="3">
+        <v>1076</v>
+      </c>
+      <c r="AS9" s="3">
+        <v>1118</v>
+      </c>
+      <c r="AT9" s="3">
+        <v>1155</v>
+      </c>
+      <c r="AU9" s="3">
+        <v>1176</v>
+      </c>
+      <c r="AV9" s="3">
+        <v>1187</v>
+      </c>
+      <c r="AW9" s="3">
+        <v>1231</v>
+      </c>
+      <c r="AX9" s="3">
+        <v>1265</v>
+      </c>
+      <c r="AY9" s="3">
+        <v>1297</v>
+      </c>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:51">
       <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="2">
         <v>7</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="2">
         <v>8</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="2">
         <v>11</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="2">
         <v>20</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="2">
         <v>25</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="2">
         <v>28</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="2">
         <v>29</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="2">
         <v>30</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J10" s="2">
         <v>33</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K10" s="2">
         <v>35</v>
       </c>
-      <c r="L10" s="6">
+      <c r="L10" s="2">
         <v>40</v>
       </c>
-      <c r="M10" s="6">
+      <c r="M10" s="2">
         <v>44</v>
       </c>
-      <c r="N10" s="6">
+      <c r="N10" s="2">
         <v>46</v>
       </c>
-      <c r="O10" s="6">
+      <c r="O10" s="2">
         <v>59</v>
       </c>
-      <c r="P10" s="6">
+      <c r="P10" s="2">
         <v>70</v>
       </c>
-      <c r="Q10" s="6">
+      <c r="Q10" s="2">
         <v>88</v>
       </c>
-      <c r="R10" s="6">
+      <c r="R10" s="2">
         <v>111</v>
       </c>
-      <c r="S10" s="6">
+      <c r="S10" s="2">
         <v>139</v>
       </c>
-      <c r="T10" s="2">
+      <c r="T10" s="1">
         <v>151</v>
       </c>
-      <c r="U10" s="2">
+      <c r="U10" s="1">
         <v>188</v>
       </c>
-      <c r="V10" s="2">
+      <c r="V10" s="1">
         <v>208</v>
       </c>
-      <c r="W10" s="2">
+      <c r="W10" s="1">
         <v>269</v>
       </c>
-      <c r="X10" s="2">
+      <c r="X10" s="1">
         <v>311</v>
       </c>
-      <c r="Y10" s="7">
+      <c r="Y10" s="3">
         <v>356</v>
       </c>
-      <c r="Z10" s="7">
+      <c r="Z10" s="3">
         <v>408</v>
       </c>
-      <c r="AA10" s="7">
+      <c r="AA10" s="3">
         <v>476</v>
       </c>
-      <c r="AB10" s="7">
+      <c r="AB10" s="3">
         <v>534</v>
       </c>
-      <c r="AC10" s="7">
+      <c r="AC10" s="3">
         <v>577</v>
       </c>
-      <c r="AD10" s="7">
+      <c r="AD10" s="3">
         <v>621</v>
       </c>
+      <c r="AE10" s="3">
+        <v>700</v>
+      </c>
+      <c r="AF10" s="3">
+        <v>747</v>
+      </c>
+      <c r="AG10" s="3">
+        <v>799</v>
+      </c>
+      <c r="AH10" s="3">
+        <v>856</v>
+      </c>
+      <c r="AI10" s="3">
+        <v>915</v>
+      </c>
+      <c r="AJ10" s="3">
+        <v>932</v>
+      </c>
+      <c r="AK10" s="3">
+        <v>989</v>
+      </c>
+      <c r="AL10" s="3">
+        <v>1040</v>
+      </c>
+      <c r="AM10" s="3">
+        <v>1107</v>
+      </c>
+      <c r="AN10" s="3">
+        <v>1172</v>
+      </c>
+      <c r="AO10" s="3">
+        <v>1239</v>
+      </c>
+      <c r="AP10" s="3">
+        <v>1344</v>
+      </c>
+      <c r="AQ10" s="3">
+        <v>1399</v>
+      </c>
+      <c r="AR10" s="3">
+        <v>1426</v>
+      </c>
+      <c r="AS10" s="3">
+        <v>1515</v>
+      </c>
+      <c r="AT10" s="3">
+        <v>1604</v>
+      </c>
+      <c r="AU10" s="3">
+        <v>1684</v>
+      </c>
+      <c r="AV10" s="3">
+        <v>1730</v>
+      </c>
+      <c r="AW10" s="3">
+        <v>1785</v>
+      </c>
+      <c r="AX10" s="3">
+        <v>1804</v>
+      </c>
+      <c r="AY10" s="3">
+        <v>1832</v>
+      </c>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:51">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="6">
-        <v>0</v>
-      </c>
-      <c r="C11" s="6">
-        <v>0</v>
-      </c>
-      <c r="D11" s="6">
-        <v>0</v>
-      </c>
-      <c r="E11" s="6">
-        <v>0</v>
-      </c>
-      <c r="F11" s="6">
-        <v>0</v>
-      </c>
-      <c r="G11" s="6">
-        <v>0</v>
-      </c>
-      <c r="H11" s="6">
-        <v>0</v>
-      </c>
-      <c r="I11" s="6">
-        <v>0</v>
-      </c>
-      <c r="J11" s="6">
-        <v>0</v>
-      </c>
-      <c r="K11" s="6">
-        <v>0</v>
-      </c>
-      <c r="L11" s="6">
-        <v>0</v>
-      </c>
-      <c r="M11" s="6">
-        <v>0</v>
-      </c>
-      <c r="N11" s="6">
-        <v>0</v>
-      </c>
-      <c r="O11" s="6">
-        <v>0</v>
-      </c>
-      <c r="P11" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="6">
-        <v>0</v>
-      </c>
-      <c r="R11" s="6">
-        <v>0</v>
-      </c>
-      <c r="S11" s="6">
-        <v>0</v>
-      </c>
-      <c r="T11" s="2">
-        <v>0</v>
-      </c>
-      <c r="U11" s="2">
-        <v>0</v>
-      </c>
-      <c r="V11" s="2">
-        <v>0</v>
-      </c>
-      <c r="W11" s="2">
-        <v>0</v>
-      </c>
-      <c r="X11" s="2">
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0</v>
+      </c>
+      <c r="M11" s="2">
+        <v>0</v>
+      </c>
+      <c r="N11" s="2">
+        <v>0</v>
+      </c>
+      <c r="O11" s="2">
+        <v>0</v>
+      </c>
+      <c r="P11" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>0</v>
+      </c>
+      <c r="R11" s="2">
+        <v>0</v>
+      </c>
+      <c r="S11" s="2">
+        <v>0</v>
+      </c>
+      <c r="T11" s="1">
+        <v>0</v>
+      </c>
+      <c r="U11" s="1">
+        <v>0</v>
+      </c>
+      <c r="V11" s="1">
+        <v>0</v>
+      </c>
+      <c r="W11" s="1">
+        <v>0</v>
+      </c>
+      <c r="X11" s="1">
         <v>2</v>
       </c>
-      <c r="Y11" s="7">
+      <c r="Y11" s="3">
         <v>2</v>
       </c>
-      <c r="Z11" s="7">
+      <c r="Z11" s="3">
         <v>2</v>
       </c>
-      <c r="AA11" s="7">
+      <c r="AA11" s="3">
         <v>4</v>
       </c>
-      <c r="AB11" s="7">
+      <c r="AB11" s="3">
         <v>4</v>
       </c>
-      <c r="AC11" s="7">
+      <c r="AC11" s="3">
         <v>4</v>
       </c>
-      <c r="AD11" s="7">
+      <c r="AD11" s="3">
         <v>4</v>
       </c>
+      <c r="AE11" s="3">
+        <v>4</v>
+      </c>
+      <c r="AF11" s="3">
+        <v>4</v>
+      </c>
+      <c r="AG11" s="3">
+        <v>4</v>
+      </c>
+      <c r="AH11" s="3">
+        <v>5</v>
+      </c>
+      <c r="AI11" s="3">
+        <v>5</v>
+      </c>
+      <c r="AJ11" s="3">
+        <v>5</v>
+      </c>
+      <c r="AK11" s="3">
+        <v>5</v>
+      </c>
+      <c r="AL11" s="3">
+        <v>5</v>
+      </c>
+      <c r="AM11" s="3">
+        <v>5</v>
+      </c>
+      <c r="AN11" s="3">
+        <v>5</v>
+      </c>
+      <c r="AO11" s="3">
+        <v>5</v>
+      </c>
+      <c r="AP11" s="3">
+        <v>5</v>
+      </c>
+      <c r="AQ11" s="3">
+        <v>6</v>
+      </c>
+      <c r="AR11" s="3">
+        <v>6</v>
+      </c>
+      <c r="AS11" s="3">
+        <v>6</v>
+      </c>
+      <c r="AT11" s="3">
+        <v>6</v>
+      </c>
+      <c r="AU11" s="3">
+        <v>6</v>
+      </c>
+      <c r="AV11" s="3">
+        <v>7</v>
+      </c>
+      <c r="AW11" s="3">
+        <v>7</v>
+      </c>
+      <c r="AX11" s="3">
+        <v>7</v>
+      </c>
+      <c r="AY11" s="3">
+        <v>7</v>
+      </c>
     </row>
-    <row r="12" spans="1:30">
+    <row r="12" spans="1:51">
       <c r="A12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="2">
         <v>2</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="2">
         <v>2</v>
       </c>
-      <c r="D12" s="6">
-        <v>6</v>
-      </c>
-      <c r="E12" s="6">
-        <v>6</v>
-      </c>
-      <c r="F12" s="6">
+      <c r="D12" s="2">
+        <v>6</v>
+      </c>
+      <c r="E12" s="2">
+        <v>6</v>
+      </c>
+      <c r="F12" s="2">
         <v>11</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="2">
         <v>11</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="2">
         <v>15</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="2">
         <v>15</v>
       </c>
-      <c r="J12" s="6">
+      <c r="J12" s="2">
         <v>16</v>
       </c>
-      <c r="K12" s="6">
+      <c r="K12" s="2">
         <v>24</v>
       </c>
-      <c r="L12" s="6">
+      <c r="L12" s="2">
         <v>24</v>
       </c>
-      <c r="M12" s="6">
+      <c r="M12" s="2">
         <v>24</v>
       </c>
-      <c r="N12" s="6">
+      <c r="N12" s="2">
         <v>24</v>
       </c>
-      <c r="O12" s="6">
+      <c r="O12" s="2">
         <v>24</v>
       </c>
-      <c r="P12" s="6">
+      <c r="P12" s="2">
         <v>24</v>
       </c>
-      <c r="Q12" s="6">
+      <c r="Q12" s="2">
         <v>24</v>
       </c>
-      <c r="R12" s="6">
+      <c r="R12" s="2">
         <v>24</v>
       </c>
-      <c r="S12" s="6">
+      <c r="S12" s="2">
         <v>24</v>
       </c>
-      <c r="T12" s="2">
+      <c r="T12" s="1">
         <v>27</v>
       </c>
-      <c r="U12" s="2">
+      <c r="U12" s="1">
         <v>27</v>
       </c>
-      <c r="V12" s="2">
+      <c r="V12" s="1">
         <v>27</v>
       </c>
-      <c r="W12" s="2">
+      <c r="W12" s="1">
         <v>29</v>
       </c>
-      <c r="X12" s="2">
+      <c r="X12" s="1">
         <v>30</v>
       </c>
-      <c r="Y12" s="7">
+      <c r="Y12" s="3">
         <v>30</v>
       </c>
-      <c r="Z12" s="7">
+      <c r="Z12" s="3">
         <v>36</v>
       </c>
-      <c r="AA12" s="7">
+      <c r="AA12" s="3">
         <v>40</v>
       </c>
-      <c r="AB12" s="7">
+      <c r="AB12" s="3">
         <v>41</v>
       </c>
-      <c r="AC12" s="7">
+      <c r="AC12" s="3">
         <v>41</v>
       </c>
-      <c r="AD12" s="7">
+      <c r="AD12" s="3">
         <v>42</v>
       </c>
+      <c r="AE12" s="3">
+        <v>43</v>
+      </c>
+      <c r="AF12" s="3">
+        <v>43</v>
+      </c>
+      <c r="AG12" s="3">
+        <v>43</v>
+      </c>
+      <c r="AH12" s="3">
+        <v>43</v>
+      </c>
+      <c r="AI12" s="3">
+        <v>43</v>
+      </c>
+      <c r="AJ12" s="3">
+        <v>45</v>
+      </c>
+      <c r="AK12" s="3">
+        <v>45</v>
+      </c>
+      <c r="AL12" s="3">
+        <v>45</v>
+      </c>
+      <c r="AM12" s="3">
+        <v>45</v>
+      </c>
+      <c r="AN12" s="3">
+        <v>45</v>
+      </c>
+      <c r="AO12" s="3">
+        <v>45</v>
+      </c>
+      <c r="AP12" s="3">
+        <v>51</v>
+      </c>
+      <c r="AQ12" s="3">
+        <v>51</v>
+      </c>
+      <c r="AR12" s="3">
+        <v>52</v>
+      </c>
+      <c r="AS12" s="3">
+        <v>54</v>
+      </c>
+      <c r="AT12" s="3">
+        <v>54</v>
+      </c>
+      <c r="AU12" s="3">
+        <v>54</v>
+      </c>
+      <c r="AV12" s="3">
+        <v>54</v>
+      </c>
+      <c r="AW12" s="3">
+        <v>54</v>
+      </c>
+      <c r="AX12" s="3">
+        <v>54</v>
+      </c>
+      <c r="AY12" s="3">
+        <v>54</v>
+      </c>
     </row>
-    <row r="13" spans="1:30">
+    <row r="13" spans="1:51">
       <c r="A13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="2">
         <v>1</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="2">
         <v>2</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="2">
         <v>4</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="2">
         <v>3</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="2">
         <v>11</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="2">
         <v>15</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="2">
         <v>17</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="2">
         <v>20</v>
       </c>
-      <c r="J13" s="6">
+      <c r="J13" s="2">
         <v>24</v>
       </c>
-      <c r="K13" s="6">
+      <c r="K13" s="2">
         <v>27</v>
       </c>
-      <c r="L13" s="6">
+      <c r="L13" s="2">
         <v>31</v>
       </c>
-      <c r="M13" s="6">
+      <c r="M13" s="2">
         <v>34</v>
       </c>
-      <c r="N13" s="6">
+      <c r="N13" s="2">
         <v>38</v>
       </c>
-      <c r="O13" s="6">
+      <c r="O13" s="2">
         <v>47</v>
       </c>
-      <c r="P13" s="6">
+      <c r="P13" s="2">
         <v>48</v>
       </c>
-      <c r="Q13" s="6">
+      <c r="Q13" s="2">
         <v>57</v>
       </c>
-      <c r="R13" s="6">
+      <c r="R13" s="2">
         <v>76</v>
       </c>
-      <c r="S13" s="6">
+      <c r="S13" s="2">
         <v>107</v>
       </c>
-      <c r="T13" s="2">
+      <c r="T13" s="1">
         <v>107</v>
       </c>
-      <c r="U13" s="2">
+      <c r="U13" s="1">
         <v>107</v>
       </c>
-      <c r="V13" s="2">
+      <c r="V13" s="1">
         <v>108</v>
       </c>
-      <c r="W13" s="2">
+      <c r="W13" s="1">
         <v>214</v>
       </c>
-      <c r="X13" s="2">
+      <c r="X13" s="1">
         <v>254</v>
       </c>
-      <c r="Y13" s="7">
+      <c r="Y13" s="3">
         <v>307</v>
       </c>
-      <c r="Z13" s="7">
+      <c r="Z13" s="3">
         <v>353</v>
       </c>
-      <c r="AA13" s="7">
+      <c r="AA13" s="3">
         <v>410</v>
       </c>
-      <c r="AB13" s="7">
+      <c r="AB13" s="3">
         <v>457</v>
       </c>
-      <c r="AC13" s="7">
+      <c r="AC13" s="3">
         <v>499</v>
       </c>
-      <c r="AD13" s="7">
+      <c r="AD13" s="3">
         <v>516</v>
       </c>
+      <c r="AE13" s="3">
+        <v>586</v>
+      </c>
+      <c r="AF13" s="3">
+        <v>667</v>
+      </c>
+      <c r="AG13" s="3">
+        <v>712</v>
+      </c>
+      <c r="AH13" s="3">
+        <v>753</v>
+      </c>
+      <c r="AI13" s="3">
+        <v>803</v>
+      </c>
+      <c r="AJ13" s="3">
+        <v>812</v>
+      </c>
+      <c r="AK13" s="3">
+        <v>826</v>
+      </c>
+      <c r="AL13" s="3">
+        <v>898</v>
+      </c>
+      <c r="AM13" s="3">
+        <v>937</v>
+      </c>
+      <c r="AN13" s="3">
+        <v>979</v>
+      </c>
+      <c r="AO13" s="3">
+        <v>1022</v>
+      </c>
+      <c r="AP13" s="3">
+        <v>1056</v>
+      </c>
+      <c r="AQ13" s="3">
+        <v>1071</v>
+      </c>
+      <c r="AR13" s="3">
+        <v>1084</v>
+      </c>
+      <c r="AS13" s="3">
+        <v>1124</v>
+      </c>
+      <c r="AT13" s="3">
+        <v>1159</v>
+      </c>
+      <c r="AU13" s="3">
+        <v>1199</v>
+      </c>
+      <c r="AV13" s="3">
+        <v>1224</v>
+      </c>
+      <c r="AW13" s="3">
+        <v>1251</v>
+      </c>
+      <c r="AX13" s="3">
+        <v>1261</v>
+      </c>
+      <c r="AY13" s="3">
+        <v>1273</v>
+      </c>
     </row>
-    <row r="14" spans="1:30">
+    <row r="14" spans="1:51">
       <c r="A14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="6">
-        <v>0</v>
-      </c>
-      <c r="C14" s="6">
-        <v>0</v>
-      </c>
-      <c r="D14" s="6">
-        <v>0</v>
-      </c>
-      <c r="E14" s="6">
-        <v>0</v>
-      </c>
-      <c r="F14" s="6">
-        <v>0</v>
-      </c>
-      <c r="G14" s="6">
-        <v>0</v>
-      </c>
-      <c r="H14" s="6">
-        <v>0</v>
-      </c>
-      <c r="I14" s="6">
-        <v>0</v>
-      </c>
-      <c r="J14" s="6">
-        <v>0</v>
-      </c>
-      <c r="K14" s="6">
-        <v>0</v>
-      </c>
-      <c r="L14" s="6">
-        <v>0</v>
-      </c>
-      <c r="M14" s="6">
-        <v>0</v>
-      </c>
-      <c r="N14" s="6">
-        <v>0</v>
-      </c>
-      <c r="O14" s="6">
-        <v>0</v>
-      </c>
-      <c r="P14" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="6">
-        <v>0</v>
-      </c>
-      <c r="R14" s="6">
-        <v>0</v>
-      </c>
-      <c r="S14" s="6">
-        <v>0</v>
-      </c>
-      <c r="T14" s="2">
-        <v>0</v>
-      </c>
-      <c r="U14" s="2">
-        <v>0</v>
-      </c>
-      <c r="V14" s="2">
-        <v>0</v>
-      </c>
-      <c r="W14" s="2">
-        <v>0</v>
-      </c>
-      <c r="X14" s="2">
+      <c r="B14" s="2">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0</v>
+      </c>
+      <c r="N14" s="2">
+        <v>0</v>
+      </c>
+      <c r="O14" s="2">
+        <v>0</v>
+      </c>
+      <c r="P14" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>0</v>
+      </c>
+      <c r="R14" s="2">
+        <v>0</v>
+      </c>
+      <c r="S14" s="2">
+        <v>0</v>
+      </c>
+      <c r="T14" s="1">
+        <v>0</v>
+      </c>
+      <c r="U14" s="1">
+        <v>0</v>
+      </c>
+      <c r="V14" s="1">
+        <v>0</v>
+      </c>
+      <c r="W14" s="1">
+        <v>0</v>
+      </c>
+      <c r="X14" s="1">
         <v>3</v>
       </c>
-      <c r="Y14" s="7">
+      <c r="Y14" s="3">
         <v>3</v>
       </c>
-      <c r="Z14" s="7">
+      <c r="Z14" s="3">
         <v>3</v>
       </c>
-      <c r="AA14" s="7">
+      <c r="AA14" s="3">
         <v>3</v>
       </c>
-      <c r="AB14" s="7">
+      <c r="AB14" s="3">
         <v>4</v>
       </c>
-      <c r="AC14" s="7">
+      <c r="AC14" s="3">
         <v>4</v>
       </c>
-      <c r="AD14" s="7">
+      <c r="AD14" s="3">
         <v>4</v>
+      </c>
+      <c r="AE14" s="3">
+        <v>4</v>
+      </c>
+      <c r="AF14" s="3">
+        <v>5</v>
+      </c>
+      <c r="AG14" s="3">
+        <v>6</v>
+      </c>
+      <c r="AH14" s="3">
+        <v>6</v>
+      </c>
+      <c r="AI14" s="3">
+        <v>6</v>
+      </c>
+      <c r="AJ14" s="3">
+        <v>6</v>
+      </c>
+      <c r="AK14" s="3">
+        <v>6</v>
+      </c>
+      <c r="AL14" s="3">
+        <v>6</v>
+      </c>
+      <c r="AM14" s="3">
+        <v>6</v>
+      </c>
+      <c r="AN14" s="3">
+        <v>6</v>
+      </c>
+      <c r="AO14" s="3">
+        <v>6</v>
+      </c>
+      <c r="AP14" s="3">
+        <v>6</v>
+      </c>
+      <c r="AQ14" s="3">
+        <v>6</v>
+      </c>
+      <c r="AR14" s="3">
+        <v>6</v>
+      </c>
+      <c r="AS14" s="3">
+        <v>6</v>
+      </c>
+      <c r="AT14" s="3">
+        <v>6</v>
+      </c>
+      <c r="AU14" s="3">
+        <v>6</v>
+      </c>
+      <c r="AV14" s="3">
+        <v>6</v>
+      </c>
+      <c r="AW14" s="3">
+        <v>6</v>
+      </c>
+      <c r="AX14" s="3">
+        <v>6</v>
+      </c>
+      <c r="AY14" s="3">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
England data now updates automatically from government website
</commit_message>
<xml_diff>
--- a/scotland_covid_data.xlsx
+++ b/scotland_covid_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -155,8 +155,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="241">
+  <cellStyleXfs count="247">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -412,7 +418,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="241">
+  <cellStyles count="247">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -533,6 +539,9 @@
     <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -653,6 +662,9 @@
     <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -982,10 +994,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CI14"/>
+  <dimension ref="A1:CK14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CE1" workbookViewId="0">
-      <selection activeCell="CJ8" sqref="CJ8"/>
+    <sheetView tabSelected="1" topLeftCell="CG1" workbookViewId="0">
+      <selection activeCell="CK14" sqref="A1:CK14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -994,7 +1006,7 @@
     <col min="25" max="25" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:87">
+    <row r="1" spans="1:89">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1256,8 +1268,14 @@
       <c r="CI1" s="3">
         <v>1066</v>
       </c>
+      <c r="CJ1" s="3">
+        <v>1071</v>
+      </c>
+      <c r="CK1" s="3">
+        <v>1076</v>
+      </c>
     </row>
-    <row r="2" spans="1:87">
+    <row r="2" spans="1:89">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -1519,8 +1537,14 @@
       <c r="CI2" s="3">
         <v>325</v>
       </c>
+      <c r="CJ2" s="3">
+        <v>325</v>
+      </c>
+      <c r="CK2" s="3">
+        <v>326</v>
+      </c>
     </row>
-    <row r="3" spans="1:87">
+    <row r="3" spans="1:89">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -1782,8 +1806,14 @@
       <c r="CI3" s="3">
         <v>260</v>
       </c>
+      <c r="CJ3" s="3">
+        <v>261</v>
+      </c>
+      <c r="CK3" s="3">
+        <v>261</v>
+      </c>
     </row>
-    <row r="4" spans="1:87">
+    <row r="4" spans="1:89">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -2045,8 +2075,14 @@
       <c r="CI4" s="3">
         <v>876</v>
       </c>
+      <c r="CJ4" s="3">
+        <v>877</v>
+      </c>
+      <c r="CK4" s="3">
+        <v>877</v>
+      </c>
     </row>
-    <row r="5" spans="1:87">
+    <row r="5" spans="1:89">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -2308,8 +2344,14 @@
       <c r="CI5" s="3">
         <v>942</v>
       </c>
+      <c r="CJ5" s="3">
+        <v>944</v>
+      </c>
+      <c r="CK5" s="3">
+        <v>946</v>
+      </c>
     </row>
-    <row r="6" spans="1:87">
+    <row r="6" spans="1:89">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -2571,8 +2613,14 @@
       <c r="CI6" s="3">
         <v>1282</v>
       </c>
+      <c r="CJ6" s="3">
+        <v>1283</v>
+      </c>
+      <c r="CK6" s="3">
+        <v>1284</v>
+      </c>
     </row>
-    <row r="7" spans="1:87">
+    <row r="7" spans="1:89">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -2834,8 +2882,14 @@
       <c r="CI7" s="3">
         <v>3954</v>
       </c>
+      <c r="CJ7" s="3">
+        <v>3961</v>
+      </c>
+      <c r="CK7" s="3">
+        <v>3968</v>
+      </c>
     </row>
-    <row r="8" spans="1:87">
+    <row r="8" spans="1:89">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -3097,8 +3151,14 @@
       <c r="CI8" s="3">
         <v>339</v>
       </c>
+      <c r="CJ8" s="3">
+        <v>338</v>
+      </c>
+      <c r="CK8" s="3">
+        <v>338</v>
+      </c>
     </row>
-    <row r="9" spans="1:87">
+    <row r="9" spans="1:89">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
@@ -3360,8 +3420,14 @@
       <c r="CI9" s="3">
         <v>1998</v>
       </c>
+      <c r="CJ9" s="3">
+        <v>2002</v>
+      </c>
+      <c r="CK9" s="3">
+        <v>2005</v>
+      </c>
     </row>
-    <row r="10" spans="1:87">
+    <row r="10" spans="1:89">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
@@ -3623,8 +3689,14 @@
       <c r="CI10" s="3">
         <v>2723</v>
       </c>
+      <c r="CJ10" s="3">
+        <v>2757</v>
+      </c>
+      <c r="CK10" s="3">
+        <v>2760</v>
+      </c>
     </row>
-    <row r="11" spans="1:87">
+    <row r="11" spans="1:89">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
@@ -3886,8 +3958,14 @@
       <c r="CI11" s="3">
         <v>8</v>
       </c>
+      <c r="CJ11" s="3">
+        <v>8</v>
+      </c>
+      <c r="CK11" s="3">
+        <v>8</v>
+      </c>
     </row>
-    <row r="12" spans="1:87">
+    <row r="12" spans="1:89">
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
@@ -4149,8 +4227,14 @@
       <c r="CI12" s="3">
         <v>54</v>
       </c>
+      <c r="CJ12" s="3">
+        <v>54</v>
+      </c>
+      <c r="CK12" s="3">
+        <v>54</v>
+      </c>
     </row>
-    <row r="13" spans="1:87">
+    <row r="13" spans="1:89">
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
@@ -4412,8 +4496,14 @@
       <c r="CI13" s="3">
         <v>1671</v>
       </c>
+      <c r="CJ13" s="3">
+        <v>1671</v>
+      </c>
+      <c r="CK13" s="3">
+        <v>1673</v>
+      </c>
     </row>
-    <row r="14" spans="1:87">
+    <row r="14" spans="1:89">
       <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
@@ -4673,6 +4763,12 @@
         <v>6</v>
       </c>
       <c r="CI14" s="3">
+        <v>6</v>
+      </c>
+      <c r="CJ14" s="3">
+        <v>6</v>
+      </c>
+      <c r="CK14" s="3">
         <v>6</v>
       </c>
     </row>

</xml_diff>